<commit_message>
conversion to spreadsheet values, mostly working: work-in-process
</commit_message>
<xml_diff>
--- a/chart.xlsx
+++ b/chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="1820" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="340" yWindow="0" windowWidth="15180" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
-  <si>
-    <t>Tick Interval</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="102">
   <si>
     <t>Use Data Set</t>
   </si>
@@ -30,15 +27,9 @@
     <t>Title</t>
   </si>
   <si>
-    <t>Overview Timeline</t>
-  </si>
-  <si>
     <t>Background Color</t>
   </si>
   <si>
-    <t>ALLCOLORS</t>
-  </si>
-  <si>
     <t>View text</t>
   </si>
   <si>
@@ -64,13 +55,283 @@
   </si>
   <si>
     <t>Phanerozoic Eon</t>
+  </si>
+  <si>
+    <t>Tick Interval (MY)</t>
+  </si>
+  <si>
+    <t>Paleo Timeline</t>
+  </si>
+  <si>
+    <t>Paleo Era</t>
+  </si>
+  <si>
+    <t>Meso Timeline</t>
+  </si>
+  <si>
+    <t>Meso Era</t>
+  </si>
+  <si>
+    <t>Neo Timeline</t>
+  </si>
+  <si>
+    <t>Neo Era</t>
+  </si>
+  <si>
+    <t>Paleozoic Timeline</t>
+  </si>
+  <si>
+    <t>Paleozoic Era</t>
+  </si>
+  <si>
+    <t>Mesozoic Timeline</t>
+  </si>
+  <si>
+    <t>Mesozoic Era</t>
+  </si>
+  <si>
+    <t>Cenozoic Timeline</t>
+  </si>
+  <si>
+    <t>Cenozoic Era</t>
+  </si>
+  <si>
+    <t>Siderian Timeline</t>
+  </si>
+  <si>
+    <t>Siderian Period</t>
+  </si>
+  <si>
+    <t>Rhyacian Timeline</t>
+  </si>
+  <si>
+    <t>Rhyacian Period</t>
+  </si>
+  <si>
+    <t>Orosirian Timeline</t>
+  </si>
+  <si>
+    <t>Orosirian Period</t>
+  </si>
+  <si>
+    <t>Statherian Timeline</t>
+  </si>
+  <si>
+    <t>Statherian Period</t>
+  </si>
+  <si>
+    <t>Calymmian Timeline</t>
+  </si>
+  <si>
+    <t>Calymmian Period</t>
+  </si>
+  <si>
+    <t>Ectasian Timeline</t>
+  </si>
+  <si>
+    <t>Ectasian Period</t>
+  </si>
+  <si>
+    <t>Stenian Timeline</t>
+  </si>
+  <si>
+    <t>Stenian Period</t>
+  </si>
+  <si>
+    <t>Tonian Timeline</t>
+  </si>
+  <si>
+    <t>Tonian Period</t>
+  </si>
+  <si>
+    <t>Cyrogenian Timeline</t>
+  </si>
+  <si>
+    <t>Cryogenian Period</t>
+  </si>
+  <si>
+    <t>Ediacaran Timeline</t>
+  </si>
+  <si>
+    <t>Ediacaran Period</t>
+  </si>
+  <si>
+    <t>Cambrian Timeline</t>
+  </si>
+  <si>
+    <t>Cambrian Period</t>
+  </si>
+  <si>
+    <t>Ordovician Timeline</t>
+  </si>
+  <si>
+    <t>Ordovician Period</t>
+  </si>
+  <si>
+    <t>Silurian Timeline</t>
+  </si>
+  <si>
+    <t>Silurian Period</t>
+  </si>
+  <si>
+    <t>Devonian Timeline</t>
+  </si>
+  <si>
+    <t>Devonian Period</t>
+  </si>
+  <si>
+    <t>Carboniferous Timeline</t>
+  </si>
+  <si>
+    <t>Carboniferous Period</t>
+  </si>
+  <si>
+    <t>Permian Timeline</t>
+  </si>
+  <si>
+    <t>Permian Period</t>
+  </si>
+  <si>
+    <t>Triassic Timeline</t>
+  </si>
+  <si>
+    <t>Triassic Period</t>
+  </si>
+  <si>
+    <t>Jurassic Timeline</t>
+  </si>
+  <si>
+    <t>Jurassic Period</t>
+  </si>
+  <si>
+    <t>Cretaceous Timeline</t>
+  </si>
+  <si>
+    <t>Cretaceous Period</t>
+  </si>
+  <si>
+    <t>Paleogene Timeline</t>
+  </si>
+  <si>
+    <t>Neogene Timeline</t>
+  </si>
+  <si>
+    <t>Neogen Period</t>
+  </si>
+  <si>
+    <t>Quaternary Timeline</t>
+  </si>
+  <si>
+    <t>Quaternary Period</t>
+  </si>
+  <si>
+    <t>Paleogene Period</t>
+  </si>
+  <si>
+    <t>CHARTBASIC</t>
+  </si>
+  <si>
+    <t>Hadean</t>
+  </si>
+  <si>
+    <t>Archean</t>
+  </si>
+  <si>
+    <t>Proterozoic</t>
+  </si>
+  <si>
+    <t>Phanerozoic</t>
+  </si>
+  <si>
+    <t>Paleo</t>
+  </si>
+  <si>
+    <t>Meso</t>
+  </si>
+  <si>
+    <t>Neo</t>
+  </si>
+  <si>
+    <t>Paleozoic</t>
+  </si>
+  <si>
+    <t>Mesozoic</t>
+  </si>
+  <si>
+    <t>Cenozoic</t>
+  </si>
+  <si>
+    <t>Siderian</t>
+  </si>
+  <si>
+    <t>Rhyacian</t>
+  </si>
+  <si>
+    <t>Orosirian</t>
+  </si>
+  <si>
+    <t>Statherian</t>
+  </si>
+  <si>
+    <t>Calymmian</t>
+  </si>
+  <si>
+    <t>Ectasian</t>
+  </si>
+  <si>
+    <t>Stenian</t>
+  </si>
+  <si>
+    <t>Tonian</t>
+  </si>
+  <si>
+    <t>Cryogenian</t>
+  </si>
+  <si>
+    <t>Ediacaran</t>
+  </si>
+  <si>
+    <t>Cambrian</t>
+  </si>
+  <si>
+    <t>Ordovician</t>
+  </si>
+  <si>
+    <t>Silurian</t>
+  </si>
+  <si>
+    <t>Devonian</t>
+  </si>
+  <si>
+    <t>Carboniferous</t>
+  </si>
+  <si>
+    <t>Permian</t>
+  </si>
+  <si>
+    <t>Triassic</t>
+  </si>
+  <si>
+    <t>Jurassic</t>
+  </si>
+  <si>
+    <t>Cretaceous</t>
+  </si>
+  <si>
+    <t>Paleogene</t>
+  </si>
+  <si>
+    <t>Neogene</t>
+  </si>
+  <si>
+    <t>Quaternary</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -88,6 +349,22 @@
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -117,10 +394,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -138,11 +419,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -472,125 +768,585 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="8.1640625" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="16" customWidth="1"/>
     <col min="3" max="3" width="24.6640625" style="6" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" customWidth="1"/>
-    <col min="5" max="5" width="45.33203125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="35" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="54">
       <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2">
-        <v>250</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
+        <v>25</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>70</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2">
-        <v>25</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
+        <v>100</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>71</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2">
         <v>100</v>
       </c>
-      <c r="B4">
-        <v>2</v>
+      <c r="B4" s="16" t="s">
+        <v>72</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="8" t="s">
+    </row>
+    <row r="5" spans="1:5" s="10" customFormat="1">
+      <c r="A5" s="9">
+        <v>25</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="2">
-        <v>100</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2">
-        <v>25</v>
-      </c>
-      <c r="B6">
-        <v>4</v>
+        <v>50</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="9" t="s">
+      <c r="D6" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" s="14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
-      <c r="C11" s="7"/>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2">
+        <v>50</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="10" customFormat="1">
+      <c r="A8" s="9">
+        <v>50</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2">
+        <v>20</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="2">
+        <v>20</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="10" customFormat="1">
+      <c r="A11" s="9">
+        <v>5</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="2">
+        <v>10</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="2">
+        <v>10</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="2">
+        <v>10</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="2">
+        <v>10</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="2">
+        <v>10</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="2">
+        <v>10</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="2">
+        <v>10</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="2">
+        <v>5</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="2">
+        <v>5</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="2">
+        <v>5</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="2">
+        <v>5</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" t="s">
+        <v>69</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="2">
+        <v>5</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="2">
+        <v>5</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" t="s">
+        <v>69</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="2">
+        <v>5</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" t="s">
+        <v>69</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="2">
+        <v>5</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" t="s">
+        <v>69</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="2">
+        <v>5</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" t="s">
+        <v>69</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="2">
+        <v>5</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" t="s">
+        <v>69</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="2">
+        <v>5</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" t="s">
+        <v>69</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="2">
+        <v>5</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D31" t="s">
+        <v>69</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="2">
+        <v>5</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" t="s">
+        <v>69</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D33" t="s">
+        <v>69</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>67</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>